<commit_message>
miscellaneous material for imports of categories and zipcodes
</commit_message>
<xml_diff>
--- a/.design/Database Scripts/Tables/Categories.xlsx
+++ b/.design/Database Scripts/Tables/Categories.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mads-\Documents\EASV\2nd-Semester-Exam\.design\Database Scripts\Tables\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaspe\Desktop\sims\2nd-Semester-Exam\.design\Database Scripts\Tables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74C54E24-E293-4591-9CFA-BCF080BBEF97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68E18273-6B2C-4F5A-A8F5-D4887019516F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{2AD1616F-6AEA-4D3C-8E18-0E525FBFEA4B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{2AD1616F-6AEA-4D3C-8E18-0E525FBFEA4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="133">
   <si>
     <t>NULL</t>
   </si>
@@ -217,6 +217,222 @@
   </si>
   <si>
     <t>Samfundsliv</t>
+  </si>
+  <si>
+    <t>Vaske sig</t>
+  </si>
+  <si>
+    <t>Gå på toilet</t>
+  </si>
+  <si>
+    <t>kropspleje</t>
+  </si>
+  <si>
+    <t>Spise</t>
+  </si>
+  <si>
+    <t>Af og påklædning</t>
+  </si>
+  <si>
+    <t>Drikke</t>
+  </si>
+  <si>
+    <t>Varetage egen sundhed</t>
+  </si>
+  <si>
+    <t>Fødeindtagelse</t>
+  </si>
+  <si>
+    <t>Udføre daglige rutiner</t>
+  </si>
+  <si>
+    <t>Skaffe sig varer og tjenesteydelser</t>
+  </si>
+  <si>
+    <t>Lave mad</t>
+  </si>
+  <si>
+    <t>Lave husligt arbejde</t>
+  </si>
+  <si>
+    <t>Ændre kropsstilling</t>
+  </si>
+  <si>
+    <t>Forflytte sig</t>
+  </si>
+  <si>
+    <t>Løfte og bære</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gå </t>
+  </si>
+  <si>
+    <t>Bevæge sig omkring</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Færden i forskellige omgivelser </t>
+  </si>
+  <si>
+    <t>Bruge transportmidler</t>
+  </si>
+  <si>
+    <t>Udholdenhed</t>
+  </si>
+  <si>
+    <t>Muskelstyrke</t>
+  </si>
+  <si>
+    <t>Tilegne sig færdigheder</t>
+  </si>
+  <si>
+    <t>Problemløsning</t>
+  </si>
+  <si>
+    <t>Anvende kommunikationsudstyr og teknikker</t>
+  </si>
+  <si>
+    <t>Orienteringsevne</t>
+  </si>
+  <si>
+    <t>Energi og handlekraft</t>
+  </si>
+  <si>
+    <t>Hukommelse</t>
+  </si>
+  <si>
+    <t>Følesesfunktioner</t>
+  </si>
+  <si>
+    <t>Overordnede kognitive funktioner</t>
+  </si>
+  <si>
+    <t>Have lønnet beskæftigelse</t>
+  </si>
+  <si>
+    <t>Problemer med personlig pleje</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Problemer med daglige aktiviteter </t>
+  </si>
+  <si>
+    <t>Problemer med mobilitet og bevæ_x0002_gelse</t>
+  </si>
+  <si>
+    <t>Problemer med væskeindtag</t>
+  </si>
+  <si>
+    <t>Problemer med fødeindtag</t>
+  </si>
+  <si>
+    <t>Uhensigtsmæssig vægtændring</t>
+  </si>
+  <si>
+    <t>Problemer med overvægt</t>
+  </si>
+  <si>
+    <t>Problemer med undervægt</t>
+  </si>
+  <si>
+    <t>Problemer med kirurgisk sår</t>
+  </si>
+  <si>
+    <t>Problemer med diabetisk sår</t>
+  </si>
+  <si>
+    <t>Problemer med cancersår</t>
+  </si>
+  <si>
+    <t>Problemer med tryksår</t>
+  </si>
+  <si>
+    <t>Problemer med arterielt sår</t>
+  </si>
+  <si>
+    <t>Problemer med venøst sår</t>
+  </si>
+  <si>
+    <t>Problemer meProblemer med traumesård blandingssår</t>
+  </si>
+  <si>
+    <t>Andre problemer med hud og slimhinder</t>
+  </si>
+  <si>
+    <t>Problemer med kommunikation</t>
+  </si>
+  <si>
+    <t>Problemer med socialt samvær</t>
+  </si>
+  <si>
+    <t>Emotionelle problemer</t>
+  </si>
+  <si>
+    <t>Problemer med misbrug</t>
+  </si>
+  <si>
+    <t>Mentale problemer</t>
+  </si>
+  <si>
+    <t>Respirationsproblemer</t>
+  </si>
+  <si>
+    <t>Cirkulationsproblemer</t>
+  </si>
+  <si>
+    <t>Problemer med seksualitet</t>
+  </si>
+  <si>
+    <t>Akutte smerter</t>
+  </si>
+  <si>
+    <t>Periodevise smerter</t>
+  </si>
+  <si>
+    <t>Kroniske smerter</t>
+  </si>
+  <si>
+    <t>Problemer med synssans</t>
+  </si>
+  <si>
+    <t>Problemer med lugtesans</t>
+  </si>
+  <si>
+    <t>Problemer med hørelse</t>
+  </si>
+  <si>
+    <t>Problemer med smagssans</t>
+  </si>
+  <si>
+    <t>Problemer med følesans</t>
+  </si>
+  <si>
+    <t>Døgnrytmeproblemer</t>
+  </si>
+  <si>
+    <t>Søvnproblemer</t>
+  </si>
+  <si>
+    <t>Problemer med hukommelse</t>
+  </si>
+  <si>
+    <t>Problemer med indsigt i behandlings_x0002_formål</t>
+  </si>
+  <si>
+    <t>Problemer med sygdomsindsigt</t>
+  </si>
+  <si>
+    <t>Kognitive problemer</t>
+  </si>
+  <si>
+    <t>Problemer med vandladning</t>
+  </si>
+  <si>
+    <t>Problemer med urininkontinens</t>
+  </si>
+  <si>
+    <t>Problemer med afføringsinkontinens</t>
+  </si>
+  <si>
+    <t>Problemer med mave og tarm</t>
   </si>
 </sst>
 </file>
@@ -232,7 +448,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -289,13 +505,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -312,7 +534,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -352,14 +574,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,54 +903,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD5FA9F7-3CA9-403D-B54B-1E4F3B708624}">
-  <dimension ref="A1:J54"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" customWidth="1"/>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" style="13" customWidth="1"/>
-    <col min="7" max="7" width="15.85546875" customWidth="1"/>
-    <col min="8" max="8" width="255.5703125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="7.5703125" hidden="1"/>
-    <col min="10" max="10" width="7" hidden="1"/>
-    <col min="11" max="16384" width="9.140625" hidden="1"/>
+    <col min="1" max="1" width="17.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" customWidth="1"/>
+    <col min="3" max="3" width="40.109375" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="15.44140625" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" style="13" customWidth="1"/>
+    <col min="7" max="7" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="255.5546875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="7" hidden="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.109375" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:10" ht="40.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15" t="s">
+      <c r="F1" s="14"/>
+      <c r="G1" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="16" t="s">
+      <c r="H1" s="15" t="s">
         <v>32</v>
       </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="9">
         <v>1</v>
       </c>
@@ -747,7 +976,7 @@
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
     </row>
-    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f>A2+1</f>
         <v>2</v>
@@ -775,7 +1004,7 @@
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
     </row>
-    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <f t="shared" ref="A4:A44" si="0">A3+1</f>
         <v>3</v>
@@ -803,7 +1032,7 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="10">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -816,11 +1045,11 @@
         <v>3</v>
       </c>
       <c r="D5" s="10">
-        <f>G2</f>
+        <f t="shared" ref="D5:D15" si="2">G2</f>
         <v>1</v>
       </c>
       <c r="E5" s="10">
-        <f>G13</f>
+        <f t="shared" ref="E5:E15" si="3">G13</f>
         <v>12</v>
       </c>
       <c r="F5" s="12"/>
@@ -834,7 +1063,7 @@
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
     </row>
-    <row r="6" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -847,11 +1076,11 @@
         <v>4</v>
       </c>
       <c r="D6" s="10">
-        <f>G3</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="E6" s="10">
-        <f>G14</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="F6" s="12"/>
@@ -865,7 +1094,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="10">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -878,11 +1107,11 @@
         <v>5</v>
       </c>
       <c r="D7" s="10">
-        <f>G4</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="E7" s="10">
-        <f>G15</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="F7" s="12"/>
@@ -896,7 +1125,7 @@
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
     </row>
-    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -909,11 +1138,11 @@
         <v>6</v>
       </c>
       <c r="D8" s="10">
-        <f>G5</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="E8" s="10">
-        <f>G16</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="F8" s="12"/>
@@ -927,7 +1156,7 @@
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
     </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="10">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -940,11 +1169,11 @@
         <v>7</v>
       </c>
       <c r="D9" s="10">
-        <f>G6</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="E9" s="10">
-        <f>G17</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="F9" s="12"/>
@@ -958,7 +1187,7 @@
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -971,11 +1200,11 @@
         <v>8</v>
       </c>
       <c r="D10" s="10">
-        <f>G7</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="E10" s="10">
-        <f>G18</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="F10" s="12"/>
@@ -989,7 +1218,7 @@
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="10">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1002,11 +1231,11 @@
         <v>9</v>
       </c>
       <c r="D11" s="10">
-        <f>G8</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="E11" s="10">
-        <f>G19</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="F11" s="12"/>
@@ -1020,7 +1249,7 @@
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="10">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1033,11 +1262,11 @@
         <v>10</v>
       </c>
       <c r="D12" s="10">
-        <f>G9</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="E12" s="10">
-        <f>G20</f>
+        <f t="shared" si="3"/>
         <v>19</v>
       </c>
       <c r="F12" s="12"/>
@@ -1051,7 +1280,7 @@
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="10">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1064,11 +1293,11 @@
         <v>11</v>
       </c>
       <c r="D13" s="10">
-        <f>G10</f>
+        <f t="shared" si="2"/>
         <v>9</v>
       </c>
       <c r="E13" s="10">
-        <f>G21</f>
+        <f t="shared" si="3"/>
         <v>20</v>
       </c>
       <c r="F13" s="12"/>
@@ -1082,7 +1311,7 @@
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="10">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1095,11 +1324,11 @@
         <v>12</v>
       </c>
       <c r="D14" s="10">
-        <f>G11</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="E14" s="10">
-        <f>G22</f>
+        <f t="shared" si="3"/>
         <v>21</v>
       </c>
       <c r="F14" s="12"/>
@@ -1113,7 +1342,7 @@
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="10">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1126,11 +1355,11 @@
         <v>13</v>
       </c>
       <c r="D15" s="10">
-        <f>G12</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="E15" s="10">
-        <f>G23</f>
+        <f t="shared" si="3"/>
         <v>22</v>
       </c>
       <c r="F15" s="12"/>
@@ -1144,7 +1373,7 @@
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="7">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1156,13 +1385,12 @@
       <c r="C16" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="D16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="F16" s="12"/>
+      <c r="D16" s="7"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="12">
+        <f>A17-A16</f>
+        <v>1</v>
+      </c>
       <c r="G16" s="11">
         <f t="shared" si="1"/>
         <v>15</v>
@@ -1173,7 +1401,7 @@
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1185,12 +1413,8 @@
       <c r="C17" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
       <c r="F17" s="12"/>
       <c r="G17" s="11">
         <f t="shared" si="1"/>
@@ -1202,7 +1426,7 @@
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="7">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1214,12 +1438,8 @@
       <c r="C18" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D18" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D18" s="7"/>
+      <c r="E18" s="7"/>
       <c r="F18" s="12"/>
       <c r="G18" s="11">
         <f t="shared" si="1"/>
@@ -1231,7 +1451,7 @@
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1243,12 +1463,8 @@
       <c r="C19" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
       <c r="F19" s="12"/>
       <c r="G19" s="11">
         <f t="shared" si="1"/>
@@ -1260,7 +1476,7 @@
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -1272,12 +1488,8 @@
       <c r="C20" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D20" s="7" t="s">
-        <v>0</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>0</v>
-      </c>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7"/>
       <c r="F20" s="12"/>
       <c r="G20" s="11">
         <f t="shared" si="1"/>
@@ -1289,7 +1501,7 @@
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="5">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1301,12 +1513,8 @@
       <c r="C21" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E21" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
       <c r="F21" s="12"/>
       <c r="G21" s="11">
         <f t="shared" si="1"/>
@@ -1318,7 +1526,7 @@
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="5">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1330,12 +1538,8 @@
       <c r="C22" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D22" s="7"/>
+      <c r="E22" s="7"/>
       <c r="F22" s="12"/>
       <c r="G22" s="11">
         <f t="shared" si="1"/>
@@ -1347,7 +1551,7 @@
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="5">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1359,12 +1563,8 @@
       <c r="C23" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E23" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
       <c r="F23" s="12"/>
       <c r="G23" s="11">
         <f t="shared" si="1"/>
@@ -1376,7 +1576,7 @@
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="5">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1388,12 +1588,8 @@
       <c r="C24" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E24" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D24" s="7"/>
+      <c r="E24" s="7"/>
       <c r="F24" s="12"/>
       <c r="G24" s="2">
         <f t="shared" si="1"/>
@@ -1405,7 +1601,7 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" s="5">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1417,12 +1613,8 @@
       <c r="C25" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E25" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
       <c r="F25" s="12"/>
       <c r="G25" s="2">
         <f t="shared" si="1"/>
@@ -1434,7 +1626,7 @@
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" s="5">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1446,12 +1638,8 @@
       <c r="C26" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D26" s="7"/>
+      <c r="E26" s="7"/>
       <c r="F26" s="12"/>
       <c r="G26" s="2">
         <f t="shared" si="1"/>
@@ -1463,7 +1651,7 @@
       <c r="I26" s="1"/>
       <c r="J26" s="1"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" s="5">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1475,12 +1663,8 @@
       <c r="C27" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E27" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
       <c r="F27" s="12"/>
       <c r="G27" s="2">
         <f t="shared" si="1"/>
@@ -1492,7 +1676,7 @@
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" s="5">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -1504,12 +1688,8 @@
       <c r="C28" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D28" s="7"/>
+      <c r="E28" s="7"/>
       <c r="F28" s="12"/>
       <c r="G28" s="2">
         <f t="shared" si="1"/>
@@ -1521,7 +1701,7 @@
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" s="5">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -1533,12 +1713,8 @@
       <c r="C29" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
       <c r="F29" s="12"/>
       <c r="G29" s="2">
         <f t="shared" si="1"/>
@@ -1550,7 +1726,7 @@
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -1562,12 +1738,8 @@
       <c r="C30" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D30" s="7"/>
+      <c r="E30" s="7"/>
       <c r="F30" s="12"/>
       <c r="G30" s="2">
         <f t="shared" si="1"/>
@@ -1579,7 +1751,7 @@
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" s="5">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -1591,12 +1763,8 @@
       <c r="C31" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
       <c r="F31" s="12"/>
       <c r="G31" s="2">
         <f t="shared" si="1"/>
@@ -1606,7 +1774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" s="5">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -1618,12 +1786,8 @@
       <c r="C32" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E32" s="5" t="s">
-        <v>0</v>
-      </c>
+      <c r="D32" s="7"/>
+      <c r="E32" s="7"/>
       <c r="F32" s="12"/>
       <c r="G32" s="2">
         <f t="shared" si="1"/>
@@ -1633,11 +1797,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="14">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" s="16">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
+      <c r="B33" s="17">
+        <v>15</v>
+      </c>
+      <c r="C33" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
       <c r="F33" s="12"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
@@ -1647,11 +1819,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="14">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="16">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
+      <c r="B34" s="17">
+        <v>15</v>
+      </c>
+      <c r="C34" s="16" t="s">
+        <v>62</v>
+      </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>33</v>
@@ -1660,11 +1840,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="14">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="16">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
+      <c r="B35" s="17">
+        <v>15</v>
+      </c>
+      <c r="C35" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>34</v>
@@ -1673,11 +1861,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="14">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" s="16">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
+      <c r="B36" s="17">
+        <v>15</v>
+      </c>
+      <c r="C36" s="16" t="s">
+        <v>65</v>
+      </c>
+      <c r="D36" s="7"/>
+      <c r="E36" s="7"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>35</v>
@@ -1686,11 +1882,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="14">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" s="16">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
+      <c r="B37" s="17">
+        <v>15</v>
+      </c>
+      <c r="C37" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>36</v>
@@ -1699,11 +1903,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="14">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="16">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
+      <c r="B38" s="17">
+        <v>15</v>
+      </c>
+      <c r="C38" s="16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D38" s="7"/>
+      <c r="E38" s="7"/>
       <c r="G38" s="2">
         <f t="shared" si="1"/>
         <v>37</v>
@@ -1712,11 +1924,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="14">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" s="16">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
+      <c r="B39" s="17">
+        <v>15</v>
+      </c>
+      <c r="C39" s="16" t="s">
+        <v>67</v>
+      </c>
+      <c r="D39" s="7"/>
+      <c r="E39" s="7"/>
       <c r="G39" s="2">
         <f t="shared" si="1"/>
         <v>38</v>
@@ -1725,11 +1945,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="14">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" s="16">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
+      <c r="B40" s="17">
+        <v>15</v>
+      </c>
+      <c r="C40" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D40" s="7"/>
+      <c r="E40" s="7"/>
       <c r="G40" s="2">
         <f t="shared" si="1"/>
         <v>39</v>
@@ -1738,11 +1966,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="14">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" s="16">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
+      <c r="B41" s="17">
+        <v>16</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>69</v>
+      </c>
+      <c r="D41" s="7"/>
+      <c r="E41" s="7"/>
       <c r="G41" s="2">
         <f t="shared" si="1"/>
         <v>40</v>
@@ -1751,11 +1987,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A42" s="14">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="16">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
+      <c r="B42" s="17">
+        <v>16</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="D42" s="7"/>
+      <c r="E42" s="7"/>
       <c r="G42" s="2">
         <f t="shared" si="1"/>
         <v>41</v>
@@ -1764,11 +2008,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="14">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" s="16">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
+      <c r="B43" s="17">
+        <v>16</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="D43" s="7"/>
+      <c r="E43" s="7"/>
       <c r="G43" s="2">
         <f t="shared" si="1"/>
         <v>42</v>
@@ -1777,11 +2029,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="14">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" s="16">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
+      <c r="B44" s="17">
+        <v>16</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="D44" s="7"/>
+      <c r="E44" s="7"/>
       <c r="G44" s="2">
         <f t="shared" si="1"/>
         <v>43</v>
@@ -1790,7 +2050,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" s="17">
+        <f>A44+1</f>
+        <v>44</v>
+      </c>
+      <c r="B45" s="17">
+        <v>17</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
       <c r="G45" s="2">
         <f t="shared" si="1"/>
         <v>44</v>
@@ -1799,7 +2071,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" s="17">
+        <f t="shared" ref="A46:A104" si="4">A45+1</f>
+        <v>45</v>
+      </c>
+      <c r="B46" s="17">
+        <v>17</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="D46" s="7"/>
+      <c r="E46" s="7"/>
       <c r="G46" s="2">
         <f t="shared" si="1"/>
         <v>45</v>
@@ -1808,7 +2092,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="17">
+        <f t="shared" si="4"/>
+        <v>46</v>
+      </c>
+      <c r="B47" s="17">
+        <v>17</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
       <c r="G47" s="2">
         <f t="shared" si="1"/>
         <v>46</v>
@@ -1817,7 +2113,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="17">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="B48" s="17">
+        <v>17</v>
+      </c>
+      <c r="C48" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="D48" s="7"/>
+      <c r="E48" s="7"/>
       <c r="G48" s="2">
         <f t="shared" si="1"/>
         <v>47</v>
@@ -1826,7 +2134,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A49" s="17">
+        <f t="shared" si="4"/>
+        <v>48</v>
+      </c>
+      <c r="B49" s="17">
+        <v>17</v>
+      </c>
+      <c r="C49" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
       <c r="G49" s="2">
         <f t="shared" si="1"/>
         <v>48</v>
@@ -1835,7 +2155,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A50" s="17">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="B50" s="17">
+        <v>17</v>
+      </c>
+      <c r="C50" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="D50" s="7"/>
+      <c r="E50" s="7"/>
       <c r="G50" s="2">
         <f t="shared" si="1"/>
         <v>49</v>
@@ -1844,7 +2176,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A51" s="17">
+        <f t="shared" si="4"/>
+        <v>50</v>
+      </c>
+      <c r="B51" s="17">
+        <v>17</v>
+      </c>
+      <c r="C51" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
       <c r="G51" s="2">
         <f t="shared" si="1"/>
         <v>50</v>
@@ -1853,7 +2197,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A52" s="17">
+        <f t="shared" si="4"/>
+        <v>51</v>
+      </c>
+      <c r="B52" s="17">
+        <v>17</v>
+      </c>
+      <c r="C52" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="D52" s="7"/>
+      <c r="E52" s="7"/>
       <c r="G52" s="2">
         <f t="shared" si="1"/>
         <v>51</v>
@@ -1862,7 +2218,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A53" s="17">
+        <f t="shared" si="4"/>
+        <v>52</v>
+      </c>
+      <c r="B53" s="17">
+        <v>17</v>
+      </c>
+      <c r="C53" s="16" t="s">
+        <v>81</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
       <c r="G53" s="2">
         <f t="shared" si="1"/>
         <v>52</v>
@@ -1871,7 +2239,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="7:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A54" s="17">
+        <f t="shared" si="4"/>
+        <v>53</v>
+      </c>
+      <c r="B54" s="17">
+        <v>18</v>
+      </c>
+      <c r="C54" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="D54" s="7"/>
+      <c r="E54" s="7"/>
       <c r="G54" s="2">
         <f t="shared" si="1"/>
         <v>53</v>
@@ -1879,6 +2259,722 @@
       <c r="H54" s="3" t="s">
         <v>0</v>
       </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A55" s="17">
+        <f t="shared" si="4"/>
+        <v>54</v>
+      </c>
+      <c r="B55" s="17">
+        <v>18</v>
+      </c>
+      <c r="C55" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A56" s="17">
+        <f t="shared" si="4"/>
+        <v>55</v>
+      </c>
+      <c r="B56" s="17">
+        <v>18</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="D56" s="7"/>
+      <c r="E56" s="7"/>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A57" s="17">
+        <f t="shared" si="4"/>
+        <v>56</v>
+      </c>
+      <c r="B57" s="17">
+        <v>18</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A58" s="17">
+        <f t="shared" si="4"/>
+        <v>57</v>
+      </c>
+      <c r="B58" s="17">
+        <v>18</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="D58" s="7"/>
+      <c r="E58" s="7"/>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A59" s="17">
+        <f t="shared" si="4"/>
+        <v>58</v>
+      </c>
+      <c r="B59" s="17">
+        <v>18</v>
+      </c>
+      <c r="C59" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A60" s="17">
+        <f t="shared" si="4"/>
+        <v>59</v>
+      </c>
+      <c r="B60" s="17">
+        <v>18</v>
+      </c>
+      <c r="C60" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="D60" s="7"/>
+      <c r="E60" s="7"/>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A61" s="17">
+        <f t="shared" si="4"/>
+        <v>60</v>
+      </c>
+      <c r="B61" s="17">
+        <v>18</v>
+      </c>
+      <c r="C61" s="16" t="s">
+        <v>89</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A62" s="17">
+        <f t="shared" si="4"/>
+        <v>61</v>
+      </c>
+      <c r="B62" s="17">
+        <v>19</v>
+      </c>
+      <c r="C62" s="16" t="s">
+        <v>90</v>
+      </c>
+      <c r="D62" s="7"/>
+      <c r="E62" s="7"/>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A63" s="18">
+        <f t="shared" si="4"/>
+        <v>62</v>
+      </c>
+      <c r="B63" s="18">
+        <v>20</v>
+      </c>
+      <c r="C63" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A64" s="18">
+        <f t="shared" si="4"/>
+        <v>63</v>
+      </c>
+      <c r="B64" s="18">
+        <v>20</v>
+      </c>
+      <c r="C64" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="7"/>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A65" s="18">
+        <f t="shared" si="4"/>
+        <v>64</v>
+      </c>
+      <c r="B65" s="18">
+        <v>21</v>
+      </c>
+      <c r="C65" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A66" s="18">
+        <f t="shared" si="4"/>
+        <v>65</v>
+      </c>
+      <c r="B66" s="18">
+        <v>22</v>
+      </c>
+      <c r="C66" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="7"/>
+      <c r="E66" s="7"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A67" s="18">
+        <f t="shared" si="4"/>
+        <v>66</v>
+      </c>
+      <c r="B67" s="18">
+        <v>22</v>
+      </c>
+      <c r="C67" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A68" s="18">
+        <f t="shared" si="4"/>
+        <v>67</v>
+      </c>
+      <c r="B68" s="18">
+        <v>22</v>
+      </c>
+      <c r="C68" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A69" s="18">
+        <f t="shared" si="4"/>
+        <v>68</v>
+      </c>
+      <c r="B69" s="18">
+        <v>22</v>
+      </c>
+      <c r="C69" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A70" s="18">
+        <f t="shared" si="4"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="18">
+        <v>22</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A71" s="18">
+        <f t="shared" si="4"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="18">
+        <v>23</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A72" s="18">
+        <f t="shared" si="4"/>
+        <v>71</v>
+      </c>
+      <c r="B72" s="18">
+        <v>23</v>
+      </c>
+      <c r="C72" s="18" t="s">
+        <v>100</v>
+      </c>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A73" s="18">
+        <f t="shared" si="4"/>
+        <v>72</v>
+      </c>
+      <c r="B73" s="18">
+        <v>23</v>
+      </c>
+      <c r="C73" s="18" t="s">
+        <v>101</v>
+      </c>
+      <c r="D73" s="7"/>
+      <c r="E73" s="7"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A74" s="18">
+        <f t="shared" si="4"/>
+        <v>73</v>
+      </c>
+      <c r="B74" s="18">
+        <v>23</v>
+      </c>
+      <c r="C74" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="D74" s="7"/>
+      <c r="E74" s="7"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A75" s="18">
+        <f t="shared" si="4"/>
+        <v>74</v>
+      </c>
+      <c r="B75" s="18">
+        <v>23</v>
+      </c>
+      <c r="C75" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="D75" s="7"/>
+      <c r="E75" s="7"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A76" s="18">
+        <f t="shared" si="4"/>
+        <v>75</v>
+      </c>
+      <c r="B76" s="18">
+        <v>23</v>
+      </c>
+      <c r="C76" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="D76" s="7"/>
+      <c r="E76" s="7"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A77" s="18">
+        <f t="shared" si="4"/>
+        <v>76</v>
+      </c>
+      <c r="B77" s="18">
+        <v>23</v>
+      </c>
+      <c r="C77" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="D77" s="7"/>
+      <c r="E77" s="7"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A78" s="18">
+        <f t="shared" si="4"/>
+        <v>77</v>
+      </c>
+      <c r="B78" s="18">
+        <v>23</v>
+      </c>
+      <c r="C78" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D78" s="7"/>
+      <c r="E78" s="7"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A79" s="18">
+        <f t="shared" si="4"/>
+        <v>78</v>
+      </c>
+      <c r="B79" s="18">
+        <v>24</v>
+      </c>
+      <c r="C79" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A80" s="18">
+        <f t="shared" si="4"/>
+        <v>79</v>
+      </c>
+      <c r="B80" s="18">
+        <v>25</v>
+      </c>
+      <c r="C80" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D80" s="7"/>
+      <c r="E80" s="7"/>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A81" s="18">
+        <f t="shared" si="4"/>
+        <v>80</v>
+      </c>
+      <c r="B81" s="18">
+        <v>25</v>
+      </c>
+      <c r="C81" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A82" s="18">
+        <f t="shared" si="4"/>
+        <v>81</v>
+      </c>
+      <c r="B82" s="18">
+        <v>25</v>
+      </c>
+      <c r="C82" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="D82" s="7"/>
+      <c r="E82" s="7"/>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A83" s="18">
+        <f t="shared" si="4"/>
+        <v>82</v>
+      </c>
+      <c r="B83" s="18">
+        <v>25</v>
+      </c>
+      <c r="C83" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A84" s="18">
+        <f t="shared" si="4"/>
+        <v>83</v>
+      </c>
+      <c r="B84" s="18">
+        <v>26</v>
+      </c>
+      <c r="C84" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D84" s="7"/>
+      <c r="E84" s="7"/>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A85" s="18">
+        <f t="shared" si="4"/>
+        <v>84</v>
+      </c>
+      <c r="B85" s="18">
+        <v>26</v>
+      </c>
+      <c r="C85" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A86" s="18">
+        <f t="shared" si="4"/>
+        <v>85</v>
+      </c>
+      <c r="B86" s="18">
+        <v>27</v>
+      </c>
+      <c r="C86" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="D86" s="7"/>
+      <c r="E86" s="7"/>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A87" s="18">
+        <f t="shared" si="4"/>
+        <v>86</v>
+      </c>
+      <c r="B87" s="18">
+        <v>28</v>
+      </c>
+      <c r="C87" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="D87" s="7"/>
+      <c r="E87" s="7"/>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A88" s="18">
+        <f t="shared" si="4"/>
+        <v>87</v>
+      </c>
+      <c r="B88" s="18">
+        <v>28</v>
+      </c>
+      <c r="C88" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="D88" s="7"/>
+      <c r="E88" s="7"/>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A89" s="18">
+        <f t="shared" si="4"/>
+        <v>88</v>
+      </c>
+      <c r="B89" s="18">
+        <v>28</v>
+      </c>
+      <c r="C89" s="18" t="s">
+        <v>117</v>
+      </c>
+      <c r="D89" s="7"/>
+      <c r="E89" s="7"/>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A90" s="18">
+        <f t="shared" si="4"/>
+        <v>89</v>
+      </c>
+      <c r="B90" s="18">
+        <v>28</v>
+      </c>
+      <c r="C90" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D90" s="7"/>
+      <c r="E90" s="7"/>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A91" s="18">
+        <f t="shared" si="4"/>
+        <v>90</v>
+      </c>
+      <c r="B91" s="18">
+        <v>28</v>
+      </c>
+      <c r="C91" s="18" t="s">
+        <v>119</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A92" s="18">
+        <f t="shared" si="4"/>
+        <v>91</v>
+      </c>
+      <c r="B92" s="18">
+        <v>28</v>
+      </c>
+      <c r="C92" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="D92" s="7"/>
+      <c r="E92" s="7"/>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A93" s="18">
+        <f t="shared" si="4"/>
+        <v>92</v>
+      </c>
+      <c r="B93" s="18">
+        <v>28</v>
+      </c>
+      <c r="C93" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="D93" s="7"/>
+      <c r="E93" s="7"/>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A94" s="18">
+        <f t="shared" si="4"/>
+        <v>93</v>
+      </c>
+      <c r="B94" s="18">
+        <v>28</v>
+      </c>
+      <c r="C94" s="18" t="s">
+        <v>122</v>
+      </c>
+      <c r="D94" s="7"/>
+      <c r="E94" s="7"/>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A95" s="18">
+        <f t="shared" si="4"/>
+        <v>94</v>
+      </c>
+      <c r="B95" s="18">
+        <v>29</v>
+      </c>
+      <c r="C95" s="18" t="s">
+        <v>123</v>
+      </c>
+      <c r="D95" s="7"/>
+      <c r="E95" s="7"/>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A96" s="18">
+        <f t="shared" si="4"/>
+        <v>95</v>
+      </c>
+      <c r="B96" s="18">
+        <v>29</v>
+      </c>
+      <c r="C96" s="18" t="s">
+        <v>124</v>
+      </c>
+      <c r="D96" s="7"/>
+      <c r="E96" s="7"/>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A97" s="18">
+        <f t="shared" si="4"/>
+        <v>96</v>
+      </c>
+      <c r="B97" s="18">
+        <v>30</v>
+      </c>
+      <c r="C97" s="18" t="s">
+        <v>125</v>
+      </c>
+      <c r="D97" s="7"/>
+      <c r="E97" s="7"/>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A98" s="18">
+        <f t="shared" si="4"/>
+        <v>97</v>
+      </c>
+      <c r="B98" s="18">
+        <v>30</v>
+      </c>
+      <c r="C98" s="18" t="s">
+        <v>126</v>
+      </c>
+      <c r="D98" s="7"/>
+      <c r="E98" s="7"/>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A99" s="18">
+        <f t="shared" si="4"/>
+        <v>98</v>
+      </c>
+      <c r="B99" s="18">
+        <v>30</v>
+      </c>
+      <c r="C99" s="18" t="s">
+        <v>127</v>
+      </c>
+      <c r="D99" s="7"/>
+      <c r="E99" s="7"/>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A100" s="18">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="B100" s="18">
+        <v>30</v>
+      </c>
+      <c r="C100" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="D100" s="7"/>
+      <c r="E100" s="7"/>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A101" s="18">
+        <f t="shared" si="4"/>
+        <v>100</v>
+      </c>
+      <c r="B101" s="18">
+        <v>31</v>
+      </c>
+      <c r="C101" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A102" s="18">
+        <f t="shared" si="4"/>
+        <v>101</v>
+      </c>
+      <c r="B102" s="18">
+        <v>31</v>
+      </c>
+      <c r="C102" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="D102" s="7"/>
+      <c r="E102" s="7"/>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A103" s="18">
+        <f t="shared" si="4"/>
+        <v>102</v>
+      </c>
+      <c r="B103" s="18">
+        <v>31</v>
+      </c>
+      <c r="C103" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A104" s="18">
+        <f t="shared" si="4"/>
+        <v>103</v>
+      </c>
+      <c r="B104" s="18">
+        <v>31</v>
+      </c>
+      <c r="C104" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D104" s="7"/>
+      <c r="E104" s="7"/>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D105" s="19"/>
+      <c r="E105" s="19"/>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D106" s="19"/>
+      <c r="E106" s="19"/>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D107" s="19"/>
+      <c r="E107" s="19"/>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D108" s="19"/>
+      <c r="E108" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>